<commit_message>
Wrangle PRISM data and write clean data to csv
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/02.1_monitoring-events-with-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/02.1_monitoring-events-with-PRISM-csv-file-name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/03_Buffelgrass CHNS/Buffelgrass_precip-variation/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{E6624D43-6562-40FF-8EBF-8675BFEB0D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC84E6C5-A29A-454A-9516-9D716CF152DE}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{E6624D43-6562-40FF-8EBF-8675BFEB0D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6812A811-E24F-48CE-8E81-959AEB3298B7}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{C691EA87-9DF1-4D7D-ACFC-EEBD4FB4EF27}"/>
   </bookViews>
@@ -282,9 +282,6 @@
     <t>PRISM_ppt_tmin_tmean_tmax_stable_4km_20221027_20231027_32.2838_-111.1922.csv</t>
   </si>
   <si>
-    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_daily_normals_32.2838_-111.1922.csv</t>
-  </si>
-  <si>
     <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_monthly_normals_32.2843_-111.1906.csv</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
   </si>
   <si>
     <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_monthly_normals_32.2111_-111.0045.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_monthly_normals_32.2838_-111.1922.csv</t>
   </si>
 </sst>
 </file>
@@ -582,6 +582,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB944EE-8876-0011-B61D-66D198252A9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12961620" y="297180"/>
+          <a:ext cx="3398520" cy="2034540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> is the list of monitoring events (unique site-transect and date), along with the corresponding CSV with PRISM data. The time period ranges from one year before the sampling date, which will be Prev_year_precip.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Precip values of each CSV are summed in 02.1.R.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -904,7 +993,7 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
@@ -912,6 +1001,7 @@
   <cols>
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5546875" bestFit="1" customWidth="1"/>
@@ -1684,7 +1774,7 @@
         <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1719,7 +1809,7 @@
         <v>37</v>
       </c>
       <c r="K23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1754,7 +1844,7 @@
         <v>37</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1789,7 +1879,7 @@
         <v>37</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1824,7 +1914,7 @@
         <v>38</v>
       </c>
       <c r="K26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1859,7 +1949,7 @@
         <v>38</v>
       </c>
       <c r="K27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1894,7 +1984,7 @@
         <v>38</v>
       </c>
       <c r="K28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1929,7 +2019,7 @@
         <v>39</v>
       </c>
       <c r="K29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1964,7 +2054,7 @@
         <v>39</v>
       </c>
       <c r="K30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1999,7 +2089,7 @@
         <v>39</v>
       </c>
       <c r="K31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2034,7 +2124,7 @@
         <v>40</v>
       </c>
       <c r="K32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -2069,7 +2159,7 @@
         <v>40</v>
       </c>
       <c r="K33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2104,7 +2194,7 @@
         <v>40</v>
       </c>
       <c r="K34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2139,7 +2229,7 @@
         <v>41</v>
       </c>
       <c r="K35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2174,7 +2264,7 @@
         <v>41</v>
       </c>
       <c r="K36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -2209,7 +2299,7 @@
         <v>41</v>
       </c>
       <c r="K37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2244,7 +2334,7 @@
         <v>42</v>
       </c>
       <c r="K38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2279,7 +2369,7 @@
         <v>42</v>
       </c>
       <c r="K39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2314,7 +2404,7 @@
         <v>42</v>
       </c>
       <c r="K40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2349,7 +2439,7 @@
         <v>43</v>
       </c>
       <c r="K41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2384,7 +2474,7 @@
         <v>43</v>
       </c>
       <c r="K42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2419,7 +2509,7 @@
         <v>43</v>
       </c>
       <c r="K43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2454,7 +2544,7 @@
         <v>44</v>
       </c>
       <c r="K44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2489,7 +2579,7 @@
         <v>44</v>
       </c>
       <c r="K45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2524,7 +2614,7 @@
         <v>44</v>
       </c>
       <c r="K46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2559,7 +2649,7 @@
         <v>44</v>
       </c>
       <c r="K47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2594,7 +2684,7 @@
         <v>45</v>
       </c>
       <c r="K48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -2629,7 +2719,7 @@
         <v>45</v>
       </c>
       <c r="K49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -2664,7 +2754,7 @@
         <v>45</v>
       </c>
       <c r="K50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2699,7 +2789,7 @@
         <v>46</v>
       </c>
       <c r="K51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -2734,7 +2824,7 @@
         <v>46</v>
       </c>
       <c r="K52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -2769,7 +2859,7 @@
         <v>46</v>
       </c>
       <c r="K53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -2804,7 +2894,7 @@
         <v>47</v>
       </c>
       <c r="K54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -2839,7 +2929,7 @@
         <v>47</v>
       </c>
       <c r="K55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -2874,7 +2964,7 @@
         <v>47</v>
       </c>
       <c r="K56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -2909,7 +2999,7 @@
         <v>48</v>
       </c>
       <c r="K57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -2944,7 +3034,7 @@
         <v>48</v>
       </c>
       <c r="K58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -2979,7 +3069,7 @@
         <v>48</v>
       </c>
       <c r="K59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -3014,7 +3104,7 @@
         <v>49</v>
       </c>
       <c r="K60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -3049,7 +3139,7 @@
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
@@ -3084,7 +3174,7 @@
         <v>49</v>
       </c>
       <c r="K62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -3119,7 +3209,7 @@
         <v>49</v>
       </c>
       <c r="K63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3154,7 +3244,7 @@
         <v>50</v>
       </c>
       <c r="K64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
@@ -3189,7 +3279,7 @@
         <v>50</v>
       </c>
       <c r="K65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -3224,7 +3314,7 @@
         <v>50</v>
       </c>
       <c r="K66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -3259,7 +3349,7 @@
         <v>51</v>
       </c>
       <c r="K67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -3294,7 +3384,7 @@
         <v>51</v>
       </c>
       <c r="K68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -3329,7 +3419,7 @@
         <v>51</v>
       </c>
       <c r="K69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -3364,7 +3454,7 @@
         <v>52</v>
       </c>
       <c r="K70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
@@ -3399,7 +3489,7 @@
         <v>52</v>
       </c>
       <c r="K71" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
@@ -3434,7 +3524,7 @@
         <v>52</v>
       </c>
       <c r="K72" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
@@ -3469,7 +3559,7 @@
         <v>52</v>
       </c>
       <c r="K73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
@@ -3504,7 +3594,7 @@
         <v>52</v>
       </c>
       <c r="K74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -3539,7 +3629,7 @@
         <v>52</v>
       </c>
       <c r="K75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
@@ -3574,7 +3664,7 @@
         <v>52</v>
       </c>
       <c r="K76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
@@ -3609,7 +3699,7 @@
         <v>52</v>
       </c>
       <c r="K77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
@@ -3644,7 +3734,7 @@
         <v>52</v>
       </c>
       <c r="K78" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
@@ -3679,7 +3769,7 @@
         <v>52</v>
       </c>
       <c r="K79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
@@ -3714,7 +3804,7 @@
         <v>53</v>
       </c>
       <c r="K80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
@@ -3749,7 +3839,7 @@
         <v>53</v>
       </c>
       <c r="K81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
@@ -3784,7 +3874,7 @@
         <v>54</v>
       </c>
       <c r="K82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
@@ -3819,12 +3909,13 @@
         <v>54</v>
       </c>
       <c r="K83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3833,12 +3924,13 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
     <col min="6" max="6" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4069,7 +4161,7 @@
         <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -4092,7 +4184,7 @@
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -4115,7 +4207,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -4138,7 +4230,7 @@
         <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -4161,7 +4253,7 @@
         <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4184,7 +4276,7 @@
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -4207,7 +4299,7 @@
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4230,7 +4322,7 @@
         <v>43</v>
       </c>
       <c r="G17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4253,7 +4345,7 @@
         <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4276,7 +4368,7 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4299,7 +4391,7 @@
         <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4322,7 +4414,7 @@
         <v>47</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4437,7 @@
         <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,7 +4460,7 @@
         <v>49</v>
       </c>
       <c r="G23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4391,7 +4483,7 @@
         <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4414,7 +4506,7 @@
         <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4437,7 +4529,7 @@
         <v>52</v>
       </c>
       <c r="G26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4460,7 +4552,7 @@
         <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4483,7 +4575,7 @@
         <v>54</v>
       </c>
       <c r="G28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>